<commit_message>
update add to cart function
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3A9C9C97-5C23-43AD-8F07-A747AA02B418}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BF8D6E61-E4C0-4D98-809D-F62A61DF1956}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="56385" yWindow="0" windowWidth="17790" windowHeight="5610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="58245" yWindow="0" windowWidth="17790" windowHeight="5610" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="42" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1507" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="469">
   <si>
     <t>Accept</t>
   </si>
@@ -1376,18 +1376,6 @@
     <t>3/4 Sleeve</t>
   </si>
   <si>
-    <t xml:space="preserve">Smart and stylish, this solid shirt features a classic cut with a button-front placket and a traditional collar. Knit side panels trim the silhouette while offering a flattering, comfortable fit. </t>
-  </si>
-  <si>
-    <t>https://dev.christopherandbanks.com/pleated-knit-to-fit-shirt-0036801530.html</t>
-  </si>
-  <si>
-    <t>Pleated Knit to Fit Shirt</t>
-  </si>
-  <si>
-    <t>030030520009544</t>
-  </si>
-  <si>
     <t>Guest
 Verify unit Price</t>
   </si>
@@ -1443,27 +1431,12 @@
     <t>P3</t>
   </si>
   <si>
-    <t xml:space="preserve">Simple and stylish, this polka-dotted tee is sure to become a casual favorite. It's crafted using soft, lightly ribbed fabric and detailed with shimmery satin trim at the neckline. </t>
-  </si>
-  <si>
-    <t>0403-NAVY</t>
-  </si>
-  <si>
-    <t>3/4 Sleeve Satin Trim Dot Print Essential Tee</t>
-  </si>
-  <si>
-    <t>10011530001753</t>
-  </si>
-  <si>
     <t>loggedin
 new-user
 new-shipping
 new-payment</t>
   </si>
   <si>
-    <t>https://dev.christopherandbanks.com/refined-everyday-denim-barely-boot-leg-petite-pant-0036789778.html</t>
-  </si>
-  <si>
     <t>AC-34</t>
   </si>
   <si>
@@ -1522,15 +1495,48 @@
   </si>
   <si>
     <t>COB-20</t>
+  </si>
+  <si>
+    <t>010011530003289</t>
+  </si>
+  <si>
+    <t>3/4 Sleeve Satin Trim Heather Essential Tee</t>
+  </si>
+  <si>
+    <t>https://dev.christopherandbanks.com/3%2F4-sleeve-satin-trim-heather-essential-tee-010011530003289.html?dwvar_010011530003289_color=0254</t>
+  </si>
+  <si>
+    <t>0254-HEATHER GREY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Satin trim at the neckline adds a touch of chic shine to this solid tee. It's crafted using lightly ribbed cotton for a super-comfy fit. </t>
+  </si>
+  <si>
+    <t>$19.95</t>
+  </si>
+  <si>
+    <t>010011530004028</t>
+  </si>
+  <si>
+    <t>Elbow Sleeve Shoulder Detail Solid Boatneck</t>
+  </si>
+  <si>
+    <t>https://dev.christopherandbanks.com/elbow-sleeve-shoulder-detail-solid-boatneck-010011530004028.html?dwvar_010011530004028_color=0126#sz=36&amp;start=37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elbow Sleeve </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nautical style is always on point, and this solid top delivers with its cuffed elbow-length sleeves, boat neckline and button detailing on the left shoulder. Pair it with colored denim for a perfectly preppy look. </t>
+  </si>
+  <si>
+    <t>$22.95</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-  </numFmts>
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -1771,7 +1777,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1961,9 +1967,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2317,7 +2320,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2355,8 +2358,8 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2393,7 +2396,9 @@
       <c r="A2" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="B2" s="20"/>
+      <c r="B2" s="17" t="s">
+        <v>49</v>
+      </c>
       <c r="C2" s="19" t="s">
         <v>123</v>
       </c>
@@ -2409,7 +2414,9 @@
       <c r="A3" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="B3" s="20"/>
+      <c r="B3" s="17" t="s">
+        <v>49</v>
+      </c>
       <c r="C3" s="19" t="s">
         <v>125</v>
       </c>
@@ -2427,7 +2434,9 @@
       <c r="A4" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="17" t="s">
+        <v>49</v>
+      </c>
       <c r="C4" s="19" t="s">
         <v>128</v>
       </c>
@@ -2445,7 +2454,9 @@
       <c r="A5" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="17" t="s">
+        <v>49</v>
+      </c>
       <c r="C5" s="19" t="s">
         <v>140</v>
       </c>
@@ -2518,7 +2529,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>51</v>
@@ -2542,13 +2553,13 @@
       </c>
       <c r="B2" s="52"/>
       <c r="C2" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F2" s="22" t="s">
         <v>292</v>
@@ -2571,13 +2582,13 @@
         <v>49</v>
       </c>
       <c r="C3" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F3" s="22" t="s">
         <v>292</v>
@@ -2600,13 +2611,13 @@
         <v>49</v>
       </c>
       <c r="C4" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F4" s="22" t="s">
         <v>292</v>
@@ -2629,13 +2640,13 @@
         <v>49</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F5" s="22" t="s">
         <v>292</v>
@@ -2658,13 +2669,13 @@
         <v>49</v>
       </c>
       <c r="C6" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F6" s="22" t="s">
         <v>292</v>
@@ -2687,13 +2698,13 @@
         <v>49</v>
       </c>
       <c r="C7" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F7" s="22" t="s">
         <v>292</v>
@@ -2716,13 +2727,13 @@
         <v>49</v>
       </c>
       <c r="C8" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F8" s="22" t="s">
         <v>292</v>
@@ -2745,13 +2756,13 @@
         <v>49</v>
       </c>
       <c r="C9" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F9" s="22" t="s">
         <v>292</v>
@@ -2774,13 +2785,13 @@
         <v>49</v>
       </c>
       <c r="C10" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F10" s="22" t="s">
         <v>292</v>
@@ -2803,13 +2814,13 @@
         <v>49</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F11" s="22" t="s">
         <v>292</v>
@@ -2832,13 +2843,13 @@
         <v>49</v>
       </c>
       <c r="C12" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F12" s="22" t="s">
         <v>292</v>
@@ -2861,13 +2872,13 @@
         <v>49</v>
       </c>
       <c r="C13" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F13" s="22" t="s">
         <v>292</v>
@@ -2890,13 +2901,13 @@
         <v>49</v>
       </c>
       <c r="C14" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F14" s="22" t="s">
         <v>292</v>
@@ -2919,13 +2930,13 @@
         <v>49</v>
       </c>
       <c r="C15" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F15" s="22" t="s">
         <v>292</v>
@@ -2948,13 +2959,13 @@
         <v>49</v>
       </c>
       <c r="C16" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F16" s="22" t="s">
         <v>292</v>
@@ -2977,13 +2988,13 @@
         <v>49</v>
       </c>
       <c r="C17" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F17" s="22" t="s">
         <v>292</v>
@@ -3006,13 +3017,13 @@
         <v>49</v>
       </c>
       <c r="C18" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F18" s="22" t="s">
         <v>292</v>
@@ -3035,13 +3046,13 @@
         <v>49</v>
       </c>
       <c r="C19" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F19" s="22" t="s">
         <v>292</v>
@@ -3064,13 +3075,13 @@
         <v>49</v>
       </c>
       <c r="C20" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F20" s="22" t="s">
         <v>292</v>
@@ -3093,13 +3104,13 @@
         <v>49</v>
       </c>
       <c r="C21" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F21" s="22" t="s">
         <v>292</v>
@@ -3122,13 +3133,13 @@
         <v>49</v>
       </c>
       <c r="C22" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F22" s="22" t="s">
         <v>292</v>
@@ -3151,13 +3162,13 @@
         <v>49</v>
       </c>
       <c r="C23" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F23" s="22" t="s">
         <v>292</v>
@@ -3180,13 +3191,13 @@
         <v>49</v>
       </c>
       <c r="C24" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F24" s="22" t="s">
         <v>292</v>
@@ -3209,13 +3220,13 @@
         <v>49</v>
       </c>
       <c r="C25" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F25" s="54" t="s">
         <v>292</v>
@@ -3238,13 +3249,13 @@
         <v>49</v>
       </c>
       <c r="C26" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F26" s="54" t="s">
         <v>292</v>
@@ -3267,13 +3278,13 @@
         <v>49</v>
       </c>
       <c r="C27" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F27" s="54" t="s">
         <v>292</v>
@@ -3296,13 +3307,13 @@
         <v>49</v>
       </c>
       <c r="C28" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F28" s="54" t="s">
         <v>292</v>
@@ -3325,13 +3336,13 @@
         <v>49</v>
       </c>
       <c r="C29" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F29" s="54" t="s">
         <v>292</v>
@@ -3354,13 +3365,13 @@
         <v>49</v>
       </c>
       <c r="C30" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F30" s="54" t="s">
         <v>292</v>
@@ -3383,13 +3394,13 @@
         <v>49</v>
       </c>
       <c r="C31" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F31" s="54" t="s">
         <v>292</v>
@@ -3412,13 +3423,13 @@
         <v>49</v>
       </c>
       <c r="C32" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F32" s="54" t="s">
         <v>292</v>
@@ -3441,13 +3452,13 @@
         <v>49</v>
       </c>
       <c r="C33" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F33" s="54" t="s">
         <v>292</v>
@@ -3464,19 +3475,19 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="52" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="B34" s="52" t="s">
         <v>49</v>
       </c>
       <c r="C34" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F34" s="54" t="s">
         <v>292</v>
@@ -3493,19 +3504,19 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="52" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="B35" s="52" t="s">
         <v>49</v>
       </c>
       <c r="C35" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F35" s="54" t="s">
         <v>292</v>
@@ -3522,19 +3533,19 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="52" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="B36" s="52" t="s">
         <v>49</v>
       </c>
       <c r="C36" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F36" s="54" t="s">
         <v>292</v>
@@ -3551,19 +3562,19 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="52" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="B37" s="52" t="s">
         <v>49</v>
       </c>
       <c r="C37" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F37" s="54" t="s">
         <v>292</v>
@@ -3580,19 +3591,19 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="52" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="B38" s="52" t="s">
         <v>49</v>
       </c>
       <c r="C38" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F38" s="54" t="s">
         <v>292</v>
@@ -3609,19 +3620,19 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="52" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="B39" s="52" t="s">
         <v>49</v>
       </c>
       <c r="C39" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F39" s="54" t="s">
         <v>292</v>
@@ -3638,19 +3649,19 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="52" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="B40" s="52" t="s">
         <v>49</v>
       </c>
       <c r="C40" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F40" s="54" t="s">
         <v>292</v>
@@ -3667,19 +3678,19 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="52" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="B41" s="52" t="s">
         <v>49</v>
       </c>
       <c r="C41" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F41" s="54" t="s">
         <v>292</v>
@@ -3696,19 +3707,19 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="52" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="B42" s="52" t="s">
         <v>49</v>
       </c>
       <c r="C42" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F42" s="54" t="s">
         <v>292</v>
@@ -3725,19 +3736,19 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="52" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="B43" s="52" t="s">
         <v>49</v>
       </c>
       <c r="C43" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F43" s="54" t="s">
         <v>292</v>
@@ -3754,19 +3765,19 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="52" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="B44" s="52" t="s">
         <v>49</v>
       </c>
       <c r="C44" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F44" s="54" t="s">
         <v>292</v>
@@ -3783,19 +3794,19 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="52" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="B45" s="52" t="s">
         <v>49</v>
       </c>
       <c r="C45" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F45" s="54" t="s">
         <v>292</v>
@@ -3812,19 +3823,19 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="52" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="B46" s="52" t="s">
         <v>49</v>
       </c>
       <c r="C46" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F46" s="54" t="s">
         <v>292</v>
@@ -3841,19 +3852,19 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="52" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="B47" s="52" t="s">
         <v>49</v>
       </c>
       <c r="C47" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F47" s="54" t="s">
         <v>292</v>
@@ -3870,19 +3881,19 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="52" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="B48" s="52" t="s">
         <v>49</v>
       </c>
       <c r="C48" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F48" s="54" t="s">
         <v>292</v>
@@ -3899,19 +3910,19 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="52" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="B49" s="52" t="s">
         <v>49</v>
       </c>
       <c r="C49" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F49" s="54" t="s">
         <v>292</v>
@@ -3928,19 +3939,19 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="52" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="B50" s="52" t="s">
         <v>49</v>
       </c>
       <c r="C50" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F50" s="54" t="s">
         <v>292</v>
@@ -3957,19 +3968,19 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="52" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
       <c r="B51" s="52" t="s">
         <v>49</v>
       </c>
       <c r="C51" s="53" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F51" s="54" t="s">
         <v>292</v>
@@ -4057,7 +4068,7 @@
         <v>348</v>
       </c>
       <c r="G2" s="64" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -5228,7 +5239,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection sqref="A1:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5312,24 +5323,24 @@
         <v>337</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="60">
+    <row r="3" spans="1:11" ht="75">
       <c r="A3" s="66" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>425</v>
+        <v>457</v>
       </c>
       <c r="C3" s="68" t="s">
-        <v>424</v>
+        <v>458</v>
       </c>
       <c r="D3" s="69" t="s">
-        <v>423</v>
-      </c>
-      <c r="E3" s="66">
-        <v>1</v>
+        <v>459</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>84</v>
       </c>
       <c r="F3" s="66" t="s">
-        <v>419</v>
+        <v>460</v>
       </c>
       <c r="G3" s="20" t="s">
         <v>335</v>
@@ -5341,30 +5352,30 @@
         <v>421</v>
       </c>
       <c r="J3" s="68" t="s">
-        <v>422</v>
-      </c>
-      <c r="K3" s="70">
-        <v>24.97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="60">
+        <v>461</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="75">
       <c r="A4" s="66" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>443</v>
+        <v>463</v>
       </c>
       <c r="C4" s="68" t="s">
-        <v>442</v>
+        <v>464</v>
       </c>
       <c r="D4" s="69" t="s">
-        <v>445</v>
-      </c>
-      <c r="E4" s="66">
-        <v>1</v>
+        <v>465</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>84</v>
       </c>
       <c r="F4" s="66" t="s">
-        <v>441</v>
+        <v>419</v>
       </c>
       <c r="G4" s="20" t="s">
         <v>335</v>
@@ -5373,18 +5384,18 @@
         <v>336</v>
       </c>
       <c r="I4" s="66" t="s">
-        <v>421</v>
+        <v>466</v>
       </c>
       <c r="J4" s="68" t="s">
-        <v>440</v>
-      </c>
-      <c r="K4" s="70">
-        <v>19.95</v>
+        <v>467</v>
+      </c>
+      <c r="K4" s="33" t="s">
+        <v>468</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{5B76A7A3-2122-40E0-9EE3-155669D5A899}"/>
+    <hyperlink ref="D3" r:id="rId1" display="https://dev.christopherandbanks.com/pleated-knit-to-fit-shirt-0036801530.html" xr:uid="{5B76A7A3-2122-40E0-9EE3-155669D5A899}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -5619,7 +5630,7 @@
         <v>42</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>43</v>
@@ -5639,7 +5650,7 @@
         <v>42</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>44</v>
@@ -5659,7 +5670,7 @@
         <v>42</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>45</v>
@@ -5679,7 +5690,7 @@
         <v>42</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>46</v>
@@ -5699,7 +5710,7 @@
         <v>42</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>47</v>
@@ -5848,7 +5859,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="30" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="G1" s="30" t="s">
         <v>51</v>
@@ -5883,13 +5894,13 @@
         <v>53</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="H2" s="32" t="s">
         <v>292</v>
@@ -5922,10 +5933,10 @@
         <v>6</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="H3" s="32" t="s">
         <v>292</v>
@@ -5952,16 +5963,16 @@
         <v>15</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="H4" s="32" t="s">
         <v>292</v>
@@ -5995,7 +6006,7 @@
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="H5" s="32" t="s">
         <v>292</v>
@@ -6025,13 +6036,13 @@
         <v>70</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="H6" s="32" t="s">
         <v>292</v>
@@ -6059,13 +6070,13 @@
         <v>66</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="H7" s="32" t="s">
         <v>292</v>
@@ -6098,10 +6109,10 @@
         <v>6</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="H8" s="32" t="s">
         <v>292</v>
@@ -6134,10 +6145,10 @@
         <v>6</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="H9" s="32" t="s">
         <v>292</v>
@@ -6170,10 +6181,10 @@
         <v>6</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="H10" s="32" t="s">
         <v>293</v>
@@ -6206,10 +6217,10 @@
         <v>6</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="H11" s="32" t="s">
         <v>293</v>
@@ -6242,10 +6253,10 @@
         <v>6</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="H12" s="32" t="s">
         <v>293</v>
@@ -6278,10 +6289,10 @@
         <v>6</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="H13" s="32" t="s">
         <v>293</v>
@@ -6312,10 +6323,10 @@
         <v>6</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="H14" s="32" t="s">
         <v>293</v>
@@ -6346,10 +6357,10 @@
         <v>6</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="H15" s="32" t="s">
         <v>293</v>
@@ -6380,10 +6391,10 @@
         <v>6</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="H16" s="32" t="s">
         <v>293</v>
@@ -6414,10 +6425,10 @@
         <v>6</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="H17" s="32" t="s">
         <v>293</v>
@@ -6448,10 +6459,10 @@
         <v>6</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="H18" s="32" t="s">
         <v>293</v>
@@ -6482,10 +6493,10 @@
         <v>6</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="H19" s="32" t="s">
         <v>293</v>
@@ -6516,10 +6527,10 @@
         <v>6</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="H20" s="32" t="s">
         <v>293</v>
@@ -6535,7 +6546,7 @@
     </row>
     <row r="21" spans="1:12" ht="60">
       <c r="A21" s="8" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>49</v>
@@ -6547,13 +6558,13 @@
         <v>130</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="H21" s="32" t="s">
         <v>292</v>
@@ -7016,7 +7027,7 @@
         <v>164</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="E2" s="33" t="s">
         <v>6</v>
@@ -7097,7 +7108,7 @@
         <v>298</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="E5" s="33" t="s">
         <v>6</v>
@@ -7119,7 +7130,7 @@
       <c r="A6" s="50" t="s">
         <v>152</v>
       </c>
-      <c r="B6" s="71"/>
+      <c r="B6" s="70"/>
       <c r="C6" s="52" t="s">
         <v>299</v>
       </c>
@@ -7150,7 +7161,7 @@
       <c r="A7" s="50" t="s">
         <v>153</v>
       </c>
-      <c r="B7" s="71"/>
+      <c r="B7" s="70"/>
       <c r="C7" s="50" t="s">
         <v>86</v>
       </c>
@@ -7267,7 +7278,7 @@
         <v>298</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="E11" s="33" t="s">
         <v>6</v>
@@ -7289,7 +7300,7 @@
       <c r="A12" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="B12" s="71"/>
+      <c r="B12" s="70"/>
       <c r="C12" s="52" t="s">
         <v>299</v>
       </c>
@@ -7320,7 +7331,7 @@
       <c r="A13" s="50" t="s">
         <v>158</v>
       </c>
-      <c r="B13" s="71"/>
+      <c r="B13" s="70"/>
       <c r="C13" s="50" t="s">
         <v>86</v>
       </c>
@@ -7358,7 +7369,7 @@
         <v>164</v>
       </c>
       <c r="D14" s="51" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="E14" s="33" t="s">
         <v>6</v>
@@ -7385,7 +7396,7 @@
         <v>164</v>
       </c>
       <c r="D15" s="51" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="E15" s="33" t="s">
         <v>6</v>
@@ -7462,7 +7473,7 @@
         <v>179</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -7476,10 +7487,10 @@
         <v>94</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -7496,7 +7507,7 @@
         <v>185</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>